<commit_message>
Added Worldpay MC, Adyen MC, standart alert, switching gateway on admin
Added Worldpay MC, Adyen MC, standart alert, switching gateway on admin
</commit_message>
<xml_diff>
--- a/CreditCards.xlsx
+++ b/CreditCards.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>CardNumber</t>
   </si>
@@ -36,10 +36,16 @@
     <t>06</t>
   </si>
   <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>042</t>
+  </si>
+  <si>
+    <t>CardholdersName</t>
+  </si>
+  <si>
+    <t>Test Card</t>
+  </si>
+  <si>
+    <t>2017</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +418,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +426,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3DS updated, accepted amount verifying added
3DS updated, accepted amount verifying added
</commit_message>
<xml_diff>
--- a/CreditCards.xlsx
+++ b/CreditCards.xlsx
@@ -4,20 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="AmericanExpress" sheetId="1" r:id="rId1"/>
     <sheet name="Visa" sheetId="2" r:id="rId2"/>
     <sheet name="MasterCard" sheetId="3" r:id="rId3"/>
     <sheet name="VisaAdyen" sheetId="4" r:id="rId4"/>
+    <sheet name="WPMC3DS" sheetId="5" r:id="rId5"/>
+    <sheet name="WPAMEX3DS" sheetId="6" r:id="rId6"/>
+    <sheet name="WPVISA3DS" sheetId="7" r:id="rId7"/>
+    <sheet name="ADYENMC3DS" sheetId="8" r:id="rId8"/>
+    <sheet name="ADYENAMEX3DS" sheetId="9" r:id="rId9"/>
+    <sheet name="ADYENVISA3DS" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
   <si>
     <t>CardNumber</t>
   </si>
@@ -65,6 +71,33 @@
   </si>
   <si>
     <t>John Doe</t>
+  </si>
+  <si>
+    <t>3DS</t>
+  </si>
+  <si>
+    <t>5555555555554444</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>5212345678901234</t>
+  </si>
+  <si>
+    <t>345177925488348</t>
+  </si>
+  <si>
+    <t>4212345678901237</t>
+  </si>
+  <si>
+    <t>7373</t>
   </si>
 </sst>
 </file>
@@ -407,7 +440,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,12 +486,71 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -584,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -638,4 +730,299 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Secure part workaround added
</commit_message>
<xml_diff>
--- a/CreditCards.xlsx
+++ b/CreditCards.xlsx
@@ -4,27 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AmericanExpress" sheetId="1" r:id="rId1"/>
     <sheet name="Visa" sheetId="2" r:id="rId2"/>
     <sheet name="MasterCard" sheetId="3" r:id="rId3"/>
-    <sheet name="VisaAdyen" sheetId="4" r:id="rId4"/>
-    <sheet name="3DSUser" sheetId="11" r:id="rId5"/>
-    <sheet name="WPMC3DS" sheetId="5" r:id="rId6"/>
-    <sheet name="WPAMEX3DS" sheetId="6" r:id="rId7"/>
-    <sheet name="WPVISA3DS" sheetId="7" r:id="rId8"/>
-    <sheet name="ADYENMC3DS" sheetId="8" r:id="rId9"/>
-    <sheet name="ADYENAMEX3DS" sheetId="9" r:id="rId10"/>
-    <sheet name="ADYENVISA3DS" sheetId="10" r:id="rId11"/>
+    <sheet name="MasterCardAdyen" sheetId="12" r:id="rId4"/>
+    <sheet name="VisaAdyen" sheetId="4" r:id="rId5"/>
+    <sheet name="3DSUser" sheetId="11" r:id="rId6"/>
+    <sheet name="WPMC3DS" sheetId="5" r:id="rId7"/>
+    <sheet name="WPAMEX3DS" sheetId="6" r:id="rId8"/>
+    <sheet name="WPVISA3DS" sheetId="7" r:id="rId9"/>
+    <sheet name="ADYENMC3DS" sheetId="8" r:id="rId10"/>
+    <sheet name="ADYENAMEX3DS" sheetId="9" r:id="rId11"/>
+    <sheet name="ADYENVISA3DS" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="27">
   <si>
     <t>CardNumber</t>
   </si>
@@ -44,18 +45,9 @@
     <t>06</t>
   </si>
   <si>
-    <t>042</t>
-  </si>
-  <si>
     <t>CardholdersName</t>
   </si>
   <si>
-    <t>Test Card</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
     <t>4444333322221111</t>
   </si>
   <si>
@@ -111,6 +103,9 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Splendor Telecom</t>
   </si>
 </sst>
 </file>
@@ -453,7 +448,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -491,15 +486,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -509,6 +504,65 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -527,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -543,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -551,15 +605,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -567,279 +621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -858,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -874,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -882,15 +664,288 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -917,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -933,7 +988,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -941,15 +996,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -976,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -992,7 +1047,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1000,15 +1055,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1051,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1059,15 +1114,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for smoke test
</commit_message>
<xml_diff>
--- a/CreditCards.xlsx
+++ b/CreditCards.xlsx
@@ -4,29 +4,30 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AmericanExpress" sheetId="1" r:id="rId1"/>
     <sheet name="Visa" sheetId="2" r:id="rId2"/>
     <sheet name="MasterCard" sheetId="3" r:id="rId3"/>
     <sheet name="MasterCardAdyen" sheetId="12" r:id="rId4"/>
-    <sheet name="VisaAdyen" sheetId="4" r:id="rId5"/>
-    <sheet name="3DSUser" sheetId="11" r:id="rId6"/>
-    <sheet name="WPMC3DS" sheetId="5" r:id="rId7"/>
-    <sheet name="WPAMEX3DS" sheetId="6" r:id="rId8"/>
-    <sheet name="WPVISA3DS" sheetId="7" r:id="rId9"/>
-    <sheet name="ADYENMC3DS" sheetId="8" r:id="rId10"/>
-    <sheet name="ADYENAMEX3DS" sheetId="9" r:id="rId11"/>
-    <sheet name="ADYENVISA3DS" sheetId="10" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId13"/>
+    <sheet name="AmexAdyen" sheetId="14" r:id="rId5"/>
+    <sheet name="VisaAdyen" sheetId="4" r:id="rId6"/>
+    <sheet name="3DSUser" sheetId="11" r:id="rId7"/>
+    <sheet name="WPMC3DS" sheetId="5" r:id="rId8"/>
+    <sheet name="WPAMEX3DS" sheetId="6" r:id="rId9"/>
+    <sheet name="WPVISA3DS" sheetId="7" r:id="rId10"/>
+    <sheet name="ADYENMC3DS" sheetId="8" r:id="rId11"/>
+    <sheet name="ADYENAMEX3DS" sheetId="9" r:id="rId12"/>
+    <sheet name="ADYENVISA3DS" sheetId="10" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="29">
   <si>
     <t>CardNumber</t>
   </si>
@@ -107,6 +108,12 @@
   </si>
   <si>
     <t>Splendor Telecom</t>
+  </si>
+  <si>
+    <t>370000000000002</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
   </si>
 </sst>
 </file>
@@ -448,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -509,7 +516,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -539,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -555,7 +562,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -606,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -627,7 +634,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -665,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,6 +689,65 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -876,7 +942,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -932,6 +998,66 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -966,7 +1092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1025,7 +1151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1082,63 +1208,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
small fixes, cleaned commented parts
</commit_message>
<xml_diff>
--- a/CreditCards.xlsx
+++ b/CreditCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="AmericanExpress" sheetId="1" r:id="rId1"/>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Creadit card updated, verifyAddedAmount updated (commented verifying, added excel adding expected and actual values)
</commit_message>
<xml_diff>
--- a/CreditCards.xlsx
+++ b/CreditCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AmericanExpress" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
     <sheet name="ADYENMC3DS" sheetId="8" r:id="rId11"/>
     <sheet name="ADYENAMEX3DS" sheetId="9" r:id="rId12"/>
     <sheet name="ADYENVISA3DS" sheetId="10" r:id="rId13"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId14"/>
+    <sheet name="DefaultRecurrect" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="29">
   <si>
     <t>CardNumber</t>
   </si>
@@ -53,9 +53,6 @@
     <t>4444333322221111</t>
   </si>
   <si>
-    <t>5454545454545454</t>
-  </si>
-  <si>
     <t>5555444433331111</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>5500 0000 0000 0004</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -494,7 +494,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -502,7 +502,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -554,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -589,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -648,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -680,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -731,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -749,28 +749,16 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -778,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -794,7 +782,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -802,7 +790,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -810,20 +798,20 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -853,7 +841,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -861,7 +849,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -869,20 +857,20 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -912,7 +900,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -920,7 +908,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -928,21 +916,20 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +943,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -972,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -980,7 +967,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -988,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -997,12 +984,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1032,7 +1019,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1040,7 +1027,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1057,53 +1044,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1111,7 +1063,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1127,7 +1079,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1135,7 +1087,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,20 +1095,56 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1186,7 +1174,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,7 +1182,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1202,7 +1190,66 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project reorganized, some files removed
</commit_message>
<xml_diff>
--- a/CreditCards.xlsx
+++ b/CreditCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="AmericanExpress" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <t>4111111111111111</t>
   </si>
   <si>
-    <t>5500 0000 0000 0004</t>
+    <t>5500000000000004</t>
   </si>
 </sst>
 </file>
@@ -751,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -869,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Euro normal Worldpay recurrent finished
</commit_message>
<xml_diff>
--- a/CreditCards.xlsx
+++ b/CreditCards.xlsx
@@ -20,7 +20,7 @@
     <sheet name="ADYENMC3DS" sheetId="8" r:id="rId11"/>
     <sheet name="ADYENAMEX3DS" sheetId="9" r:id="rId12"/>
     <sheet name="ADYENVISA3DS" sheetId="10" r:id="rId13"/>
-    <sheet name="DefaultRecurrect" sheetId="13" r:id="rId14"/>
+    <sheet name="DefaultRecurrent" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -752,7 +752,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>